<commit_message>
add scaling factor = sqrt(3) for all input DC powers / P_ac=sqrt(3)*U_ac*I_ac*cos_phi / P_dc=V_dc*I_dc --> for V_dc=U_ac: P_dc=sqrt(3)*P_ac add scaling factor for all output DC powers (P, Q, and losses) --> function update_dc_results add length of lines in output plots change settings to launch scenario 1 --> if user sizes storager, scenario 1 is not launched, and therefore not evaluated
</commit_message>
<xml_diff>
--- a/catalogue_converter.xlsx
+++ b/catalogue_converter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I43680\Documents\pythonProjects\dc_design_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320BB125-7DE4-4835-BEEA-165D0785ECEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77A3406-600A-4B9C-AB83-1B0A9FF92104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B310722E-489A-462F-B946-DDE9E21437D8}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="25">
   <si>
     <t>Converter type</t>
   </si>
@@ -146,7 +146,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -269,7 +269,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -283,14 +283,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -300,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -313,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -648,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE1DD91-E4BB-483E-AD34-9CF8C62E28B1}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -989,37 +989,37 @@
       </c>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2250</v>
+      </c>
+      <c r="D10" s="5">
+        <v>400</v>
+      </c>
+      <c r="E10" s="5">
+        <v>700</v>
+      </c>
+      <c r="F10" s="5">
+        <v>60</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="5">
         <v>17</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="7">
-        <v>500</v>
-      </c>
-      <c r="D10" s="7">
-        <v>700</v>
-      </c>
-      <c r="E10" s="5">
-        <v>150</v>
-      </c>
-      <c r="F10" s="5">
-        <v>20</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="5">
-        <v>10</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="L10" s="5"/>
     </row>
@@ -1040,7 +1040,7 @@
         <v>150</v>
       </c>
       <c r="F11" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G11" s="6">
         <v>0.97499999999999998</v>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>150</v>
       </c>
       <c r="F12" s="5">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G12" s="6">
         <v>0.97499999999999998</v>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>150</v>
       </c>
       <c r="F13" s="5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G13" s="6">
         <v>0.97499999999999998</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>13</v>
@@ -1142,7 +1142,7 @@
         <v>150</v>
       </c>
       <c r="F14" s="5">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G14" s="6">
         <v>0.97499999999999998</v>
@@ -1176,7 +1176,7 @@
         <v>150</v>
       </c>
       <c r="F15" s="5">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G15" s="6">
         <v>0.97499999999999998</v>
@@ -1210,7 +1210,7 @@
         <v>150</v>
       </c>
       <c r="F16" s="5">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G16" s="6">
         <v>0.97499999999999998</v>
@@ -1244,7 +1244,7 @@
         <v>150</v>
       </c>
       <c r="F17" s="5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G17" s="6">
         <v>0.97499999999999998</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>13</v>
@@ -1278,7 +1278,7 @@
         <v>150</v>
       </c>
       <c r="F18" s="5">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G18" s="6">
         <v>0.97499999999999998</v>
@@ -1287,17 +1287,17 @@
         <v>21</v>
       </c>
       <c r="I18" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>13</v>
@@ -1312,7 +1312,7 @@
         <v>150</v>
       </c>
       <c r="F19" s="5">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G19" s="6">
         <v>0.97499999999999998</v>
@@ -1321,11 +1321,11 @@
         <v>21</v>
       </c>
       <c r="I19" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L19" s="5"/>
     </row>
@@ -1346,7 +1346,7 @@
         <v>150</v>
       </c>
       <c r="F20" s="5">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G20" s="6">
         <v>0.97499999999999998</v>
@@ -1380,7 +1380,7 @@
         <v>150</v>
       </c>
       <c r="F21" s="5">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="G21" s="6">
         <v>0.97499999999999998</v>
@@ -1389,32 +1389,32 @@
         <v>21</v>
       </c>
       <c r="I21" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="7">
+        <v>500</v>
+      </c>
+      <c r="D22" s="7">
+        <v>700</v>
+      </c>
+      <c r="E22" s="5">
+        <v>150</v>
+      </c>
+      <c r="F22" s="5">
         <v>22</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="7">
-        <v>500</v>
-      </c>
-      <c r="D22" s="7">
-        <v>350</v>
-      </c>
-      <c r="E22" s="5">
-        <v>48</v>
-      </c>
-      <c r="F22" s="5">
-        <v>0.5</v>
       </c>
       <c r="G22" s="6">
         <v>0.97499999999999998</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>13</v>
@@ -1442,13 +1442,13 @@
         <v>500</v>
       </c>
       <c r="D23" s="7">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="E23" s="5">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F23" s="5">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="G23" s="6">
         <v>0.97499999999999998</v>
@@ -1457,11 +1457,11 @@
         <v>21</v>
       </c>
       <c r="I23" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="L23" s="5"/>
     </row>
@@ -1482,7 +1482,7 @@
         <v>48</v>
       </c>
       <c r="F24" s="5">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="G24" s="6">
         <v>0.97499999999999998</v>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L24" s="5"/>
     </row>
@@ -1510,13 +1510,13 @@
         <v>500</v>
       </c>
       <c r="D25" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E25" s="5">
         <v>48</v>
       </c>
       <c r="F25" s="5">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G25" s="6">
         <v>0.97499999999999998</v>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L25" s="5"/>
     </row>
@@ -1544,13 +1544,13 @@
         <v>500</v>
       </c>
       <c r="D26" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E26" s="5">
-        <v>350</v>
+        <v>48</v>
       </c>
       <c r="F26" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G26" s="6">
         <v>0.97499999999999998</v>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L26" s="5"/>
     </row>
@@ -1581,10 +1581,10 @@
         <v>700</v>
       </c>
       <c r="E27" s="5">
-        <v>350</v>
+        <v>48</v>
       </c>
       <c r="F27" s="5">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G27" s="6">
         <v>0.97499999999999998</v>
@@ -1618,7 +1618,7 @@
         <v>350</v>
       </c>
       <c r="F28" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G28" s="6">
         <v>0.97499999999999998</v>
@@ -1652,7 +1652,7 @@
         <v>350</v>
       </c>
       <c r="F29" s="5">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G29" s="6">
         <v>0.97499999999999998</v>
@@ -1661,17 +1661,17 @@
         <v>21</v>
       </c>
       <c r="I29" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>13</v>
@@ -1680,33 +1680,32 @@
         <v>500</v>
       </c>
       <c r="D30" s="7">
+        <v>700</v>
+      </c>
+      <c r="E30" s="5">
         <v>350</v>
       </c>
-      <c r="E30" s="5">
-        <v>48</v>
-      </c>
       <c r="F30" s="5">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="G30" s="6">
-        <f>G29*0.99</f>
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I30" s="5">
         <v>5</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>13</v>
@@ -1715,26 +1714,26 @@
         <v>500</v>
       </c>
       <c r="D31" s="7">
+        <v>700</v>
+      </c>
+      <c r="E31" s="5">
         <v>350</v>
       </c>
-      <c r="E31" s="5">
-        <v>48</v>
-      </c>
       <c r="F31" s="5">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="G31" s="6">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I31" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="L31" s="5"/>
     </row>
@@ -1755,9 +1754,10 @@
         <v>48</v>
       </c>
       <c r="F32" s="5">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="G32" s="6">
+        <f>G31*0.99</f>
         <v>0.96524999999999994</v>
       </c>
       <c r="H32" s="5" t="s">
@@ -1783,13 +1783,13 @@
         <v>500</v>
       </c>
       <c r="D33" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E33" s="5">
         <v>48</v>
       </c>
       <c r="F33" s="5">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G33" s="6">
         <v>0.96524999999999994</v>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L33" s="5"/>
     </row>
@@ -1817,17 +1817,16 @@
         <v>500</v>
       </c>
       <c r="D34" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E34" s="5">
-        <v>350</v>
+        <v>48</v>
       </c>
       <c r="F34" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G34" s="6">
-        <f>G33*0.99</f>
-        <v>0.95559749999999999</v>
+        <v>0.96524999999999994</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>24</v>
@@ -1837,7 +1836,7 @@
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L34" s="5"/>
     </row>
@@ -1855,10 +1854,10 @@
         <v>700</v>
       </c>
       <c r="E35" s="5">
-        <v>350</v>
+        <v>48</v>
       </c>
       <c r="F35" s="5">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G35" s="6">
         <v>0.96524999999999994</v>
@@ -1892,31 +1891,32 @@
         <v>350</v>
       </c>
       <c r="F36" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G36" s="6">
-        <v>0.96524999999999994</v>
+        <f>G35*0.99</f>
+        <v>0.95559749999999999</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I36" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="10">
+      <c r="B37" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="7">
         <v>500</v>
       </c>
       <c r="D37" s="7">
@@ -1926,94 +1926,90 @@
         <v>350</v>
       </c>
       <c r="F37" s="5">
+        <v>15</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" s="5">
+        <v>5</v>
+      </c>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5">
+        <v>10</v>
+      </c>
+      <c r="L37" s="5"/>
+    </row>
+    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="7">
+        <v>500</v>
+      </c>
+      <c r="D38" s="7">
+        <v>700</v>
+      </c>
+      <c r="E38" s="5">
+        <v>350</v>
+      </c>
+      <c r="F38" s="5">
+        <v>20</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="5">
+        <v>10</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5">
+        <v>35</v>
+      </c>
+      <c r="L38" s="5"/>
+    </row>
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="10">
+        <v>500</v>
+      </c>
+      <c r="D39" s="7">
+        <v>700</v>
+      </c>
+      <c r="E39" s="5">
+        <v>350</v>
+      </c>
+      <c r="F39" s="5">
         <v>50</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G39" s="12">
         <v>0.96524999999999994</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I37" s="5">
-        <v>10</v>
-      </c>
-      <c r="J37" s="11"/>
-      <c r="K37" s="5">
+      <c r="I39" s="5">
+        <v>10</v>
+      </c>
+      <c r="J39" s="11"/>
+      <c r="K39" s="5">
         <v>35</v>
       </c>
-      <c r="L37" s="11"/>
-    </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="18">
-        <v>850</v>
-      </c>
-      <c r="D38" s="18">
-        <v>400</v>
-      </c>
-      <c r="E38" s="18">
-        <v>700</v>
-      </c>
-      <c r="F38" s="18">
-        <v>100</v>
-      </c>
-      <c r="G38" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H38" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I38" s="18">
-        <v>17</v>
-      </c>
-      <c r="J38" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="K38" s="18">
-        <v>250</v>
-      </c>
-      <c r="L38" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="18">
-        <v>1000</v>
-      </c>
-      <c r="D39" s="18">
-        <v>400</v>
-      </c>
-      <c r="E39" s="18">
-        <v>700</v>
-      </c>
-      <c r="F39" s="18">
-        <v>125</v>
-      </c>
-      <c r="G39" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I39" s="18">
-        <v>17</v>
-      </c>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18">
-        <v>250</v>
-      </c>
-      <c r="L39" s="18"/>
+      <c r="L39" s="11"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
@@ -2022,8 +2018,8 @@
       <c r="B40" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="20">
-        <v>1250</v>
+      <c r="C40" s="18">
+        <v>850</v>
       </c>
       <c r="D40" s="18">
         <v>400</v>
@@ -2032,7 +2028,7 @@
         <v>700</v>
       </c>
       <c r="F40" s="18">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G40" s="19">
         <v>0.97499999999999998</v>
@@ -2043,11 +2039,15 @@
       <c r="I40" s="18">
         <v>17</v>
       </c>
-      <c r="J40" s="18"/>
+      <c r="J40" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="K40" s="18">
         <v>250</v>
       </c>
-      <c r="L40" s="18"/>
+      <c r="L40" s="18" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
@@ -2056,8 +2056,8 @@
       <c r="B41" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="20">
-        <v>1500</v>
+      <c r="C41" s="18">
+        <v>1000</v>
       </c>
       <c r="D41" s="18">
         <v>400</v>
@@ -2066,7 +2066,7 @@
         <v>700</v>
       </c>
       <c r="F41" s="18">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="G41" s="19">
         <v>0.97499999999999998</v>
@@ -2085,13 +2085,13 @@
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="18">
-        <v>1500</v>
+      <c r="C42" s="20">
+        <v>1250</v>
       </c>
       <c r="D42" s="18">
         <v>400</v>
@@ -2100,37 +2100,32 @@
         <v>700</v>
       </c>
       <c r="F42" s="18">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G42" s="19">
-        <f>G41*0.99</f>
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I42" s="18">
         <v>17</v>
       </c>
-      <c r="J42" s="18" t="s">
-        <v>14</v>
-      </c>
+      <c r="J42" s="18"/>
       <c r="K42" s="18">
         <v>250</v>
       </c>
-      <c r="L42" s="18" t="s">
-        <v>15</v>
-      </c>
+      <c r="L42" s="18"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C43" s="20">
-        <v>1750</v>
+        <v>1500</v>
       </c>
       <c r="D43" s="18">
         <v>400</v>
@@ -2139,13 +2134,13 @@
         <v>700</v>
       </c>
       <c r="F43" s="18">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="G43" s="19">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I43" s="18">
         <v>17</v>
@@ -2163,8 +2158,8 @@
       <c r="B44" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="20">
-        <v>2000</v>
+      <c r="C44" s="18">
+        <v>1500</v>
       </c>
       <c r="D44" s="18">
         <v>400</v>
@@ -2173,9 +2168,10 @@
         <v>700</v>
       </c>
       <c r="F44" s="18">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G44" s="19">
+        <f>G43*0.99</f>
         <v>0.96524999999999994</v>
       </c>
       <c r="H44" s="18" t="s">
@@ -2184,11 +2180,15 @@
       <c r="I44" s="18">
         <v>17</v>
       </c>
-      <c r="J44" s="18"/>
+      <c r="J44" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="K44" s="18">
         <v>250</v>
       </c>
-      <c r="L44" s="18"/>
+      <c r="L44" s="18" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
@@ -2198,7 +2198,7 @@
         <v>20</v>
       </c>
       <c r="C45" s="20">
-        <v>2250</v>
+        <v>1750</v>
       </c>
       <c r="D45" s="18">
         <v>400</v>
@@ -2207,7 +2207,7 @@
         <v>700</v>
       </c>
       <c r="F45" s="18">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="G45" s="19">
         <v>0.96524999999999994</v>
@@ -2225,70 +2225,70 @@
       <c r="L45" s="18"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="20">
+        <v>2000</v>
+      </c>
+      <c r="D46" s="18">
+        <v>400</v>
+      </c>
+      <c r="E46" s="18">
+        <v>700</v>
+      </c>
+      <c r="F46" s="18">
+        <v>150</v>
+      </c>
+      <c r="G46" s="19">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" s="18">
         <v>17</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="20">
-        <v>500</v>
-      </c>
-      <c r="D46" s="20">
-        <v>700</v>
-      </c>
-      <c r="E46" s="18">
-        <v>150</v>
-      </c>
-      <c r="F46" s="18">
-        <v>20</v>
-      </c>
-      <c r="G46" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I46" s="18">
-        <v>10</v>
       </c>
       <c r="J46" s="18"/>
       <c r="K46" s="18">
-        <v>35</v>
+        <v>250</v>
       </c>
       <c r="L46" s="18"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="20">
+        <v>2250</v>
+      </c>
+      <c r="D47" s="18">
+        <v>400</v>
+      </c>
+      <c r="E47" s="18">
+        <v>700</v>
+      </c>
+      <c r="F47" s="18">
+        <v>175</v>
+      </c>
+      <c r="G47" s="19">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="18">
         <v>17</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="20">
-        <v>500</v>
-      </c>
-      <c r="D47" s="20">
-        <v>700</v>
-      </c>
-      <c r="E47" s="18">
-        <v>150</v>
-      </c>
-      <c r="F47" s="18">
-        <v>30</v>
-      </c>
-      <c r="G47" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I47" s="18">
-        <v>10</v>
       </c>
       <c r="J47" s="18"/>
       <c r="K47" s="18">
-        <v>35</v>
+        <v>250</v>
       </c>
       <c r="L47" s="18"/>
     </row>
@@ -2309,7 +2309,7 @@
         <v>150</v>
       </c>
       <c r="F48" s="18">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G48" s="19">
         <v>0.97499999999999998</v>
@@ -2343,7 +2343,7 @@
         <v>150</v>
       </c>
       <c r="F49" s="18">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G49" s="19">
         <v>0.97499999999999998</v>
@@ -2362,7 +2362,7 @@
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B50" s="13" t="s">
         <v>20</v>
@@ -2377,7 +2377,7 @@
         <v>150</v>
       </c>
       <c r="F50" s="18">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G50" s="19">
         <v>0.97499999999999998</v>
@@ -2396,7 +2396,7 @@
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B51" s="13" t="s">
         <v>20</v>
@@ -2411,7 +2411,7 @@
         <v>150</v>
       </c>
       <c r="F51" s="18">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G51" s="19">
         <v>0.97499999999999998</v>
@@ -2445,7 +2445,7 @@
         <v>150</v>
       </c>
       <c r="F52" s="18">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G52" s="19">
         <v>0.97499999999999998</v>
@@ -2479,7 +2479,7 @@
         <v>150</v>
       </c>
       <c r="F53" s="18">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G53" s="19">
         <v>0.97499999999999998</v>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>20</v>
@@ -2513,7 +2513,7 @@
         <v>150</v>
       </c>
       <c r="F54" s="18">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G54" s="19">
         <v>0.97499999999999998</v>
@@ -2522,17 +2522,17 @@
         <v>21</v>
       </c>
       <c r="I54" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J54" s="18"/>
       <c r="K54" s="18">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L54" s="18"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B55" s="13" t="s">
         <v>20</v>
@@ -2547,7 +2547,7 @@
         <v>150</v>
       </c>
       <c r="F55" s="18">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G55" s="19">
         <v>0.97499999999999998</v>
@@ -2556,11 +2556,11 @@
         <v>21</v>
       </c>
       <c r="I55" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J55" s="18"/>
       <c r="K55" s="18">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L55" s="18"/>
     </row>
@@ -2581,7 +2581,7 @@
         <v>150</v>
       </c>
       <c r="F56" s="18">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G56" s="19">
         <v>0.97499999999999998</v>
@@ -2615,7 +2615,7 @@
         <v>150</v>
       </c>
       <c r="F57" s="18">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="G57" s="19">
         <v>0.97499999999999998</v>
@@ -2624,32 +2624,32 @@
         <v>21</v>
       </c>
       <c r="I57" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J57" s="18"/>
       <c r="K57" s="18">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="L57" s="18"/>
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="20">
+        <v>500</v>
+      </c>
+      <c r="D58" s="20">
+        <v>700</v>
+      </c>
+      <c r="E58" s="18">
+        <v>150</v>
+      </c>
+      <c r="F58" s="18">
         <v>22</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C58" s="20">
-        <v>500</v>
-      </c>
-      <c r="D58" s="20">
-        <v>350</v>
-      </c>
-      <c r="E58" s="18">
-        <v>48</v>
-      </c>
-      <c r="F58" s="18">
-        <v>0.5</v>
       </c>
       <c r="G58" s="19">
         <v>0.97499999999999998</v>
@@ -2668,7 +2668,7 @@
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>20</v>
@@ -2677,13 +2677,13 @@
         <v>500</v>
       </c>
       <c r="D59" s="20">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="E59" s="18">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F59" s="18">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="G59" s="19">
         <v>0.97499999999999998</v>
@@ -2692,11 +2692,11 @@
         <v>21</v>
       </c>
       <c r="I59" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J59" s="18"/>
       <c r="K59" s="18">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="L59" s="18"/>
     </row>
@@ -2717,7 +2717,7 @@
         <v>48</v>
       </c>
       <c r="F60" s="18">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="G60" s="19">
         <v>0.97499999999999998</v>
@@ -2730,7 +2730,7 @@
       </c>
       <c r="J60" s="18"/>
       <c r="K60" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L60" s="18"/>
     </row>
@@ -2745,13 +2745,13 @@
         <v>500</v>
       </c>
       <c r="D61" s="20">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E61" s="18">
         <v>48</v>
       </c>
       <c r="F61" s="18">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G61" s="19">
         <v>0.97499999999999998</v>
@@ -2764,7 +2764,7 @@
       </c>
       <c r="J61" s="18"/>
       <c r="K61" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L61" s="18"/>
     </row>
@@ -2779,13 +2779,13 @@
         <v>500</v>
       </c>
       <c r="D62" s="20">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E62" s="18">
-        <v>350</v>
+        <v>48</v>
       </c>
       <c r="F62" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G62" s="19">
         <v>0.97499999999999998</v>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="J62" s="18"/>
       <c r="K62" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L62" s="18"/>
     </row>
@@ -2816,10 +2816,10 @@
         <v>700</v>
       </c>
       <c r="E63" s="18">
-        <v>350</v>
+        <v>48</v>
       </c>
       <c r="F63" s="18">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G63" s="19">
         <v>0.97499999999999998</v>
@@ -2853,7 +2853,7 @@
         <v>350</v>
       </c>
       <c r="F64" s="18">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G64" s="19">
         <v>0.97499999999999998</v>
@@ -2887,7 +2887,7 @@
         <v>350</v>
       </c>
       <c r="F65" s="18">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G65" s="19">
         <v>0.97499999999999998</v>
@@ -2896,17 +2896,17 @@
         <v>21</v>
       </c>
       <c r="I65" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J65" s="18"/>
       <c r="K65" s="18">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="L65" s="18"/>
     </row>
     <row r="66" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>20</v>
@@ -2915,33 +2915,32 @@
         <v>500</v>
       </c>
       <c r="D66" s="20">
+        <v>700</v>
+      </c>
+      <c r="E66" s="18">
         <v>350</v>
       </c>
-      <c r="E66" s="18">
-        <v>48</v>
-      </c>
       <c r="F66" s="18">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="G66" s="19">
-        <f>G65*0.99</f>
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I66" s="18">
         <v>5</v>
       </c>
       <c r="J66" s="18"/>
       <c r="K66" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L66" s="18"/>
     </row>
     <row r="67" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>20</v>
@@ -2950,26 +2949,26 @@
         <v>500</v>
       </c>
       <c r="D67" s="20">
+        <v>700</v>
+      </c>
+      <c r="E67" s="18">
         <v>350</v>
       </c>
-      <c r="E67" s="18">
-        <v>48</v>
-      </c>
       <c r="F67" s="18">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="G67" s="19">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I67" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J67" s="18"/>
       <c r="K67" s="18">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="L67" s="18"/>
     </row>
@@ -2990,9 +2989,10 @@
         <v>48</v>
       </c>
       <c r="F68" s="18">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="G68" s="19">
+        <f>G67*0.99</f>
         <v>0.96524999999999994</v>
       </c>
       <c r="H68" s="18" t="s">
@@ -3018,13 +3018,13 @@
         <v>500</v>
       </c>
       <c r="D69" s="20">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E69" s="18">
         <v>48</v>
       </c>
       <c r="F69" s="18">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G69" s="19">
         <v>0.96524999999999994</v>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="J69" s="18"/>
       <c r="K69" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L69" s="18"/>
     </row>
@@ -3052,17 +3052,16 @@
         <v>500</v>
       </c>
       <c r="D70" s="20">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E70" s="18">
-        <v>350</v>
+        <v>48</v>
       </c>
       <c r="F70" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G70" s="19">
-        <f>G69*0.99</f>
-        <v>0.95559749999999999</v>
+        <v>0.96524999999999994</v>
       </c>
       <c r="H70" s="18" t="s">
         <v>24</v>
@@ -3072,7 +3071,7 @@
       </c>
       <c r="J70" s="18"/>
       <c r="K70" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L70" s="18"/>
     </row>
@@ -3083,32 +3082,32 @@
       <c r="B71" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="22">
-        <v>500</v>
-      </c>
-      <c r="D71" s="22">
-        <v>700</v>
-      </c>
-      <c r="E71" s="23">
-        <v>350</v>
-      </c>
-      <c r="F71" s="23">
-        <v>15</v>
-      </c>
-      <c r="G71" s="24">
+      <c r="C71" s="20">
+        <v>500</v>
+      </c>
+      <c r="D71" s="20">
+        <v>700</v>
+      </c>
+      <c r="E71" s="18">
+        <v>48</v>
+      </c>
+      <c r="F71" s="18">
+        <v>11</v>
+      </c>
+      <c r="G71" s="19">
         <v>0.96524999999999994</v>
       </c>
-      <c r="H71" s="23" t="s">
+      <c r="H71" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I71" s="23">
-        <v>5</v>
-      </c>
-      <c r="J71" s="23"/>
-      <c r="K71" s="23">
-        <v>10</v>
-      </c>
-      <c r="L71" s="23"/>
+      <c r="I71" s="18">
+        <v>5</v>
+      </c>
+      <c r="J71" s="18"/>
+      <c r="K71" s="18">
+        <v>10</v>
+      </c>
+      <c r="L71" s="18"/>
     </row>
     <row r="72" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="21" t="s">
@@ -3117,66 +3116,135 @@
       <c r="B72" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C72" s="16">
-        <v>500</v>
-      </c>
-      <c r="D72" s="16">
-        <v>700</v>
-      </c>
-      <c r="E72" s="14">
+      <c r="C72" s="20">
+        <v>500</v>
+      </c>
+      <c r="D72" s="20">
+        <v>700</v>
+      </c>
+      <c r="E72" s="18">
         <v>350</v>
       </c>
-      <c r="F72" s="14">
-        <v>20</v>
-      </c>
-      <c r="G72" s="15">
+      <c r="F72" s="18">
+        <v>10</v>
+      </c>
+      <c r="G72" s="19">
+        <f>G71*0.99</f>
+        <v>0.95559749999999999</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I72" s="18">
+        <v>5</v>
+      </c>
+      <c r="J72" s="18"/>
+      <c r="K72" s="18">
+        <v>10</v>
+      </c>
+      <c r="L72" s="18"/>
+    </row>
+    <row r="73" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C73" s="22">
+        <v>500</v>
+      </c>
+      <c r="D73" s="22">
+        <v>700</v>
+      </c>
+      <c r="E73" s="23">
+        <v>350</v>
+      </c>
+      <c r="F73" s="23">
+        <v>15</v>
+      </c>
+      <c r="G73" s="24">
         <v>0.96524999999999994</v>
       </c>
-      <c r="H72" s="14" t="s">
+      <c r="H73" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="I72" s="14">
-        <v>10</v>
-      </c>
-      <c r="J72" s="14"/>
-      <c r="K72" s="14">
+      <c r="I73" s="23">
+        <v>5</v>
+      </c>
+      <c r="J73" s="23"/>
+      <c r="K73" s="23">
+        <v>10</v>
+      </c>
+      <c r="L73" s="23"/>
+    </row>
+    <row r="74" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" s="16">
+        <v>500</v>
+      </c>
+      <c r="D74" s="16">
+        <v>700</v>
+      </c>
+      <c r="E74" s="14">
+        <v>350</v>
+      </c>
+      <c r="F74" s="14">
+        <v>20</v>
+      </c>
+      <c r="G74" s="15">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H74" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I74" s="14">
+        <v>10</v>
+      </c>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14">
         <v>35</v>
       </c>
-      <c r="L72" s="14"/>
-    </row>
-    <row r="73" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="25" t="s">
+      <c r="L74" s="14"/>
+    </row>
+    <row r="75" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B73" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C73" s="16">
-        <v>500</v>
-      </c>
-      <c r="D73" s="16">
-        <v>700</v>
-      </c>
-      <c r="E73" s="14">
+      <c r="B75" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C75" s="16">
+        <v>500</v>
+      </c>
+      <c r="D75" s="16">
+        <v>700</v>
+      </c>
+      <c r="E75" s="14">
         <v>350</v>
       </c>
-      <c r="F73" s="14">
+      <c r="F75" s="14">
         <v>50</v>
       </c>
-      <c r="G73" s="15">
+      <c r="G75" s="15">
         <v>0.96524999999999994</v>
       </c>
-      <c r="H73" s="14" t="s">
+      <c r="H75" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I73" s="14">
-        <v>10</v>
-      </c>
-      <c r="J73" s="14"/>
-      <c r="K73" s="14">
+      <c r="I75" s="14">
+        <v>10</v>
+      </c>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14">
         <v>35</v>
       </c>
-      <c r="L73" s="14"/>
+      <c r="L75" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3186,17 +3254,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a656bf76-cca4-4796-b3e3-9ff4debad9ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3f4d043c-ef99-408b-9086-307465b47223" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3205,7 +3262,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005D48458B7DF5B44891BF6C8B708F036C" ma:contentTypeVersion="15" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="6ec72bf5cc41951886dd851de9b63939">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a656bf76-cca4-4796-b3e3-9ff4debad9ca" xmlns:ns3="3f4d043c-ef99-408b-9086-307465b47223" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="619265aacb58e563d368a43a0aeb056e" ns2:_="" ns3:_="">
     <xsd:import namespace="a656bf76-cca4-4796-b3e3-9ff4debad9ca"/>
@@ -3440,18 +3497,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4198C07A-8C8E-492A-A3EC-F4C24C93A879}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a656bf76-cca4-4796-b3e3-9ff4debad9ca"/>
-    <ds:schemaRef ds:uri="3f4d043c-ef99-408b-9086-307465b47223"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a656bf76-cca4-4796-b3e3-9ff4debad9ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3f4d043c-ef99-408b-9086-307465b47223" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00F984FD-7FB1-4E24-9C54-AB8DB7C9EB67}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -3459,7 +3516,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F970F1C-4AA8-4790-8FBB-C76490AE23B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3476,4 +3533,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4198C07A-8C8E-492A-A3EC-F4C24C93A879}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a656bf76-cca4-4796-b3e3-9ff4debad9ca"/>
+    <ds:schemaRef ds:uri="3f4d043c-ef99-408b-9086-307465b47223"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update droop_correction function in utilities_load_flow.py : add associated linked converter , in addition to direclty linked --> for get_voltage_bus and get_droop_curve update catalogue_converter by adding converters that we will need in the demos
</commit_message>
<xml_diff>
--- a/catalogue_converter.xlsx
+++ b/catalogue_converter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I43680\Documents\pythonProjects\dc_design_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77A3406-600A-4B9C-AB83-1B0A9FF92104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6D0018-704D-49A3-B446-BC8E48D3E8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B310722E-489A-462F-B946-DDE9E21437D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B310722E-489A-462F-B946-DDE9E21437D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Converters" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="26">
   <si>
     <t>Converter type</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>[10;91.6], [30; 95.5], [60; 96], [100; 96.5]</t>
+  </si>
+  <si>
+    <t>DC/AC Converter</t>
   </si>
 </sst>
 </file>
@@ -648,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE1DD91-E4BB-483E-AD34-9CF8C62E28B1}">
-  <dimension ref="A1:L75"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -850,25 +853,24 @@
     </row>
     <row r="6" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5">
-        <v>1500</v>
+      <c r="C6" s="7">
+        <v>2250</v>
       </c>
       <c r="D6" s="5">
         <v>400</v>
       </c>
       <c r="E6" s="5">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="F6" s="5">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G6" s="6">
-        <f>G5*0.99</f>
         <v>0.96524999999999994</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -877,25 +879,21 @@
       <c r="I6" s="5">
         <v>17</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="J6" s="5"/>
       <c r="K6" s="5">
-        <v>250</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="7">
-        <v>1750</v>
+        <v>2250</v>
       </c>
       <c r="D7" s="5">
         <v>400</v>
@@ -904,7 +902,7 @@
         <v>700</v>
       </c>
       <c r="F7" s="5">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="G7" s="6">
         <v>0.96524999999999994</v>
@@ -917,28 +915,28 @@
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="7">
-        <v>2000</v>
+        <v>2250</v>
       </c>
       <c r="D8" s="5">
         <v>400</v>
       </c>
       <c r="E8" s="5">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="F8" s="5">
-        <v>150</v>
+        <v>11</v>
       </c>
       <c r="G8" s="6">
         <v>0.96524999999999994</v>
@@ -951,7 +949,7 @@
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="L8" s="5"/>
     </row>
@@ -962,8 +960,8 @@
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="7">
-        <v>2250</v>
+      <c r="C9" s="5">
+        <v>1500</v>
       </c>
       <c r="D9" s="5">
         <v>400</v>
@@ -972,9 +970,10 @@
         <v>700</v>
       </c>
       <c r="F9" s="5">
-        <v>175</v>
+        <v>100</v>
       </c>
       <c r="G9" s="6">
+        <f>G5*0.99</f>
         <v>0.96524999999999994</v>
       </c>
       <c r="H9" s="5" t="s">
@@ -983,11 +982,15 @@
       <c r="I9" s="5">
         <v>17</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="K9" s="5">
         <v>250</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -997,7 +1000,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="7">
-        <v>2250</v>
+        <v>1750</v>
       </c>
       <c r="D10" s="5">
         <v>400</v>
@@ -1006,7 +1009,7 @@
         <v>700</v>
       </c>
       <c r="F10" s="5">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="G10" s="6">
         <v>0.96524999999999994</v>
@@ -1019,115 +1022,115 @@
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2000</v>
+      </c>
+      <c r="D11" s="5">
+        <v>400</v>
+      </c>
+      <c r="E11" s="5">
+        <v>700</v>
+      </c>
+      <c r="F11" s="5">
+        <v>150</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="5">
         <v>17</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="7">
-        <v>500</v>
-      </c>
-      <c r="D11" s="7">
-        <v>700</v>
-      </c>
-      <c r="E11" s="5">
-        <v>150</v>
-      </c>
-      <c r="F11" s="5">
-        <v>20</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="5">
-        <v>10</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5">
-        <v>35</v>
+        <v>250</v>
       </c>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="7">
+        <v>2250</v>
+      </c>
+      <c r="D12" s="5">
+        <v>400</v>
+      </c>
+      <c r="E12" s="5">
+        <v>700</v>
+      </c>
+      <c r="F12" s="5">
+        <v>175</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="5">
         <v>17</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="7">
-        <v>500</v>
-      </c>
-      <c r="D12" s="7">
-        <v>700</v>
-      </c>
-      <c r="E12" s="5">
-        <v>150</v>
-      </c>
-      <c r="F12" s="5">
-        <v>30</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="5">
-        <v>10</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5">
-        <v>35</v>
+        <v>250</v>
       </c>
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2250</v>
+      </c>
+      <c r="D13" s="5">
+        <v>400</v>
+      </c>
+      <c r="E13" s="5">
+        <v>700</v>
+      </c>
+      <c r="F13" s="5">
+        <v>60</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="5">
         <v>17</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="7">
-        <v>500</v>
-      </c>
-      <c r="D13" s="7">
-        <v>700</v>
-      </c>
-      <c r="E13" s="5">
-        <v>150</v>
-      </c>
-      <c r="F13" s="5">
-        <v>40</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="5">
-        <v>10</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>13</v>
@@ -1136,13 +1139,13 @@
         <v>500</v>
       </c>
       <c r="D14" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E14" s="5">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="F14" s="5">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="G14" s="6">
         <v>0.97499999999999998</v>
@@ -1151,17 +1154,17 @@
         <v>21</v>
       </c>
       <c r="I14" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>13</v>
@@ -1170,13 +1173,13 @@
         <v>500</v>
       </c>
       <c r="D15" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E15" s="5">
         <v>150</v>
       </c>
       <c r="F15" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G15" s="6">
         <v>0.97499999999999998</v>
@@ -1189,13 +1192,13 @@
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>13</v>
@@ -1210,7 +1213,7 @@
         <v>150</v>
       </c>
       <c r="F16" s="5">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G16" s="6">
         <v>0.97499999999999998</v>
@@ -1223,13 +1226,13 @@
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>13</v>
@@ -1244,7 +1247,7 @@
         <v>150</v>
       </c>
       <c r="F17" s="5">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G17" s="6">
         <v>0.97499999999999998</v>
@@ -1257,13 +1260,13 @@
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>13</v>
@@ -1278,7 +1281,7 @@
         <v>150</v>
       </c>
       <c r="F18" s="5">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G18" s="6">
         <v>0.97499999999999998</v>
@@ -1297,7 +1300,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>13</v>
@@ -1312,7 +1315,7 @@
         <v>150</v>
       </c>
       <c r="F19" s="5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G19" s="6">
         <v>0.97499999999999998</v>
@@ -1329,9 +1332,9 @@
       </c>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>13</v>
@@ -1346,7 +1349,7 @@
         <v>150</v>
       </c>
       <c r="F20" s="5">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G20" s="6">
         <v>0.97499999999999998</v>
@@ -1355,17 +1358,17 @@
         <v>21</v>
       </c>
       <c r="I20" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>13</v>
@@ -1380,7 +1383,7 @@
         <v>150</v>
       </c>
       <c r="F21" s="5">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G21" s="6">
         <v>0.97499999999999998</v>
@@ -1389,17 +1392,17 @@
         <v>21</v>
       </c>
       <c r="I21" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>13</v>
@@ -1414,7 +1417,7 @@
         <v>150</v>
       </c>
       <c r="F22" s="5">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G22" s="6">
         <v>0.97499999999999998</v>
@@ -1423,17 +1426,17 @@
         <v>21</v>
       </c>
       <c r="I22" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>13</v>
@@ -1442,13 +1445,13 @@
         <v>500</v>
       </c>
       <c r="D23" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E23" s="5">
         <v>150</v>
       </c>
       <c r="F23" s="5">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="G23" s="6">
         <v>0.97499999999999998</v>
@@ -1467,7 +1470,7 @@
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>13</v>
@@ -1476,13 +1479,13 @@
         <v>500</v>
       </c>
       <c r="D24" s="7">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="E24" s="5">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F24" s="5">
-        <v>0.5</v>
+        <v>11</v>
       </c>
       <c r="G24" s="6">
         <v>0.97499999999999998</v>
@@ -1491,17 +1494,17 @@
         <v>21</v>
       </c>
       <c r="I24" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>13</v>
@@ -1510,13 +1513,13 @@
         <v>500</v>
       </c>
       <c r="D25" s="7">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="E25" s="5">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F25" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G25" s="6">
         <v>0.97499999999999998</v>
@@ -1525,17 +1528,17 @@
         <v>21</v>
       </c>
       <c r="I25" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>13</v>
@@ -1544,13 +1547,13 @@
         <v>500</v>
       </c>
       <c r="D26" s="7">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="E26" s="5">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F26" s="5">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G26" s="6">
         <v>0.97499999999999998</v>
@@ -1559,17 +1562,17 @@
         <v>21</v>
       </c>
       <c r="I26" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>13</v>
@@ -1581,10 +1584,10 @@
         <v>700</v>
       </c>
       <c r="E27" s="5">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F27" s="5">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="G27" s="6">
         <v>0.97499999999999998</v>
@@ -1593,17 +1596,17 @@
         <v>21</v>
       </c>
       <c r="I27" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>13</v>
@@ -1615,10 +1618,10 @@
         <v>700</v>
       </c>
       <c r="E28" s="5">
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="F28" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G28" s="6">
         <v>0.97499999999999998</v>
@@ -1627,17 +1630,17 @@
         <v>21</v>
       </c>
       <c r="I28" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>13</v>
@@ -1649,10 +1652,10 @@
         <v>700</v>
       </c>
       <c r="E29" s="5">
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="F29" s="5">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G29" s="6">
         <v>0.97499999999999998</v>
@@ -1671,7 +1674,7 @@
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>13</v>
@@ -1680,13 +1683,13 @@
         <v>500</v>
       </c>
       <c r="D30" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E30" s="5">
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="F30" s="5">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G30" s="6">
         <v>0.97499999999999998</v>
@@ -1705,7 +1708,7 @@
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>13</v>
@@ -1717,10 +1720,10 @@
         <v>700</v>
       </c>
       <c r="E31" s="5">
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="F31" s="5">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="G31" s="6">
         <v>0.97499999999999998</v>
@@ -1729,17 +1732,17 @@
         <v>21</v>
       </c>
       <c r="I31" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>13</v>
@@ -1751,30 +1754,29 @@
         <v>350</v>
       </c>
       <c r="E32" s="5">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F32" s="5">
-        <v>0.5</v>
+        <v>22</v>
       </c>
       <c r="G32" s="6">
-        <f>G31*0.99</f>
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I32" s="5">
         <v>5</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>13</v>
@@ -1783,32 +1785,32 @@
         <v>500</v>
       </c>
       <c r="D33" s="7">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="E33" s="5">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F33" s="5">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="G33" s="6">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I33" s="5">
         <v>5</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>13</v>
@@ -1817,32 +1819,32 @@
         <v>500</v>
       </c>
       <c r="D34" s="7">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="E34" s="5">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F34" s="5">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G34" s="6">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I34" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>13</v>
@@ -1851,19 +1853,19 @@
         <v>500</v>
       </c>
       <c r="D35" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E35" s="5">
         <v>48</v>
       </c>
       <c r="F35" s="5">
-        <v>11</v>
+        <v>0.5</v>
       </c>
       <c r="G35" s="6">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I35" s="5">
         <v>5</v>
@@ -1876,7 +1878,7 @@
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>13</v>
@@ -1885,33 +1887,32 @@
         <v>500</v>
       </c>
       <c r="D36" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E36" s="5">
-        <v>350</v>
+        <v>48</v>
       </c>
       <c r="F36" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G36" s="6">
-        <f>G35*0.99</f>
-        <v>0.95559749999999999</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I36" s="5">
         <v>5</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>13</v>
@@ -1920,32 +1921,32 @@
         <v>500</v>
       </c>
       <c r="D37" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E37" s="5">
-        <v>350</v>
+        <v>48</v>
       </c>
       <c r="F37" s="5">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G37" s="6">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I37" s="5">
         <v>5</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>13</v>
@@ -1954,737 +1955,734 @@
         <v>500</v>
       </c>
       <c r="D38" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="E38" s="5">
-        <v>350</v>
+        <v>48</v>
       </c>
       <c r="F38" s="5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G38" s="6">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I38" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5">
+        <v>5</v>
+      </c>
+      <c r="L38" s="5"/>
+    </row>
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="7">
+        <v>500</v>
+      </c>
+      <c r="D39" s="7">
+        <v>350</v>
+      </c>
+      <c r="E39" s="5">
+        <v>48</v>
+      </c>
+      <c r="F39" s="5">
+        <v>6</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="5">
+        <v>5</v>
+      </c>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5">
+        <v>5</v>
+      </c>
+      <c r="L39" s="5"/>
+    </row>
+    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="7">
+        <v>500</v>
+      </c>
+      <c r="D40" s="7">
+        <v>350</v>
+      </c>
+      <c r="E40" s="5">
+        <v>48</v>
+      </c>
+      <c r="F40" s="5">
+        <v>11</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="5">
+        <v>5</v>
+      </c>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5">
+        <v>10</v>
+      </c>
+      <c r="L40" s="5"/>
+    </row>
+    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="7">
+        <v>500</v>
+      </c>
+      <c r="D41" s="7">
+        <v>700</v>
+      </c>
+      <c r="E41" s="5">
+        <v>350</v>
+      </c>
+      <c r="F41" s="5">
+        <v>11</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" s="5">
+        <v>5</v>
+      </c>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5">
+        <v>10</v>
+      </c>
+      <c r="L41" s="5"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="7">
+        <v>500</v>
+      </c>
+      <c r="D42" s="7">
+        <v>700</v>
+      </c>
+      <c r="E42" s="5">
+        <v>350</v>
+      </c>
+      <c r="F42" s="5">
+        <v>10</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="5">
+        <v>5</v>
+      </c>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5">
+        <v>10</v>
+      </c>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="7">
+        <v>500</v>
+      </c>
+      <c r="D43" s="7">
+        <v>700</v>
+      </c>
+      <c r="E43" s="5">
+        <v>350</v>
+      </c>
+      <c r="F43" s="5">
+        <v>15</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" s="5">
+        <v>5</v>
+      </c>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5">
+        <v>10</v>
+      </c>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="7">
+        <v>500</v>
+      </c>
+      <c r="D44" s="7">
+        <v>700</v>
+      </c>
+      <c r="E44" s="5">
+        <v>350</v>
+      </c>
+      <c r="F44" s="5">
+        <v>20</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="5">
+        <v>5</v>
+      </c>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5">
+        <v>10</v>
+      </c>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="7">
+        <v>500</v>
+      </c>
+      <c r="D45" s="7">
+        <v>700</v>
+      </c>
+      <c r="E45" s="5">
+        <v>350</v>
+      </c>
+      <c r="F45" s="5">
+        <v>50</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" s="5">
+        <v>10</v>
+      </c>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5">
         <v>35</v>
       </c>
-      <c r="L38" s="5"/>
-    </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="10">
-        <v>500</v>
-      </c>
-      <c r="D39" s="7">
-        <v>700</v>
-      </c>
-      <c r="E39" s="5">
-        <v>350</v>
-      </c>
-      <c r="F39" s="5">
+      <c r="B46" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="7">
+        <v>500</v>
+      </c>
+      <c r="D46" s="7">
+        <v>350</v>
+      </c>
+      <c r="E46" s="5">
+        <v>48</v>
+      </c>
+      <c r="F46" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G46" s="6">
+        <f>G45*0.99</f>
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" s="5">
+        <v>5</v>
+      </c>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5">
+        <v>5</v>
+      </c>
+      <c r="L46" s="5"/>
+    </row>
+    <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="7">
+        <v>500</v>
+      </c>
+      <c r="D47" s="7">
+        <v>350</v>
+      </c>
+      <c r="E47" s="5">
+        <v>48</v>
+      </c>
+      <c r="F47" s="5">
+        <v>1</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="5">
+        <v>5</v>
+      </c>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5">
+        <v>5</v>
+      </c>
+      <c r="L47" s="5"/>
+    </row>
+    <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="7">
+        <v>500</v>
+      </c>
+      <c r="D48" s="7">
+        <v>350</v>
+      </c>
+      <c r="E48" s="5">
+        <v>48</v>
+      </c>
+      <c r="F48" s="5">
+        <v>3</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="5">
+        <v>5</v>
+      </c>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5">
+        <v>5</v>
+      </c>
+      <c r="L48" s="5"/>
+    </row>
+    <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="7">
+        <v>500</v>
+      </c>
+      <c r="D49" s="7">
+        <v>350</v>
+      </c>
+      <c r="E49" s="5">
+        <v>48</v>
+      </c>
+      <c r="F49" s="5">
+        <v>5</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="5">
+        <v>5</v>
+      </c>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5">
+        <v>5</v>
+      </c>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="7">
+        <v>500</v>
+      </c>
+      <c r="D50" s="7">
+        <v>350</v>
+      </c>
+      <c r="E50" s="5">
+        <v>48</v>
+      </c>
+      <c r="F50" s="5">
+        <v>6</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" s="5">
+        <v>5</v>
+      </c>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5">
+        <v>5</v>
+      </c>
+      <c r="L50" s="5"/>
+    </row>
+    <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="7">
+        <v>500</v>
+      </c>
+      <c r="D51" s="7">
+        <v>350</v>
+      </c>
+      <c r="E51" s="5">
+        <v>48</v>
+      </c>
+      <c r="F51" s="5">
+        <v>11</v>
+      </c>
+      <c r="G51" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I51" s="5">
+        <v>5</v>
+      </c>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5">
+        <v>10</v>
+      </c>
+      <c r="L51" s="5"/>
+    </row>
+    <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="7">
+        <v>500</v>
+      </c>
+      <c r="D52" s="7">
+        <v>700</v>
+      </c>
+      <c r="E52" s="5">
+        <v>350</v>
+      </c>
+      <c r="F52" s="5">
+        <v>11</v>
+      </c>
+      <c r="G52" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I52" s="5">
+        <v>5</v>
+      </c>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5">
+        <v>10</v>
+      </c>
+      <c r="L52" s="5"/>
+    </row>
+    <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="7">
+        <v>500</v>
+      </c>
+      <c r="D53" s="7">
+        <v>700</v>
+      </c>
+      <c r="E53" s="5">
+        <v>350</v>
+      </c>
+      <c r="F53" s="5">
+        <v>10</v>
+      </c>
+      <c r="G53" s="6">
+        <f>G52*0.99</f>
+        <v>0.95559749999999999</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I53" s="5">
+        <v>5</v>
+      </c>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5">
+        <v>10</v>
+      </c>
+      <c r="L53" s="5"/>
+    </row>
+    <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="7">
+        <v>500</v>
+      </c>
+      <c r="D54" s="7">
+        <v>700</v>
+      </c>
+      <c r="E54" s="5">
+        <v>350</v>
+      </c>
+      <c r="F54" s="5">
+        <v>15</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I54" s="5">
+        <v>5</v>
+      </c>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5">
+        <v>10</v>
+      </c>
+      <c r="L54" s="5"/>
+    </row>
+    <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="7">
+        <v>500</v>
+      </c>
+      <c r="D55" s="7">
+        <v>700</v>
+      </c>
+      <c r="E55" s="5">
+        <v>350</v>
+      </c>
+      <c r="F55" s="5">
+        <v>20</v>
+      </c>
+      <c r="G55" s="6">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I55" s="5">
+        <v>10</v>
+      </c>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5">
+        <v>35</v>
+      </c>
+      <c r="L55" s="5"/>
+    </row>
+    <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="10">
+        <v>500</v>
+      </c>
+      <c r="D56" s="7">
+        <v>700</v>
+      </c>
+      <c r="E56" s="5">
+        <v>350</v>
+      </c>
+      <c r="F56" s="5">
         <v>50</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G56" s="12">
         <v>0.96524999999999994</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H56" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="5">
-        <v>10</v>
-      </c>
-      <c r="J39" s="11"/>
-      <c r="K39" s="5">
+      <c r="I56" s="5">
+        <v>10</v>
+      </c>
+      <c r="J56" s="11"/>
+      <c r="K56" s="5">
         <v>35</v>
       </c>
-      <c r="L39" s="11"/>
-    </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
+      <c r="L56" s="11"/>
+    </row>
+    <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="18">
+      <c r="B57" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="18">
         <v>850</v>
       </c>
-      <c r="D40" s="18">
+      <c r="D57" s="18">
         <v>400</v>
       </c>
-      <c r="E40" s="18">
-        <v>700</v>
-      </c>
-      <c r="F40" s="18">
+      <c r="E57" s="18">
+        <v>700</v>
+      </c>
+      <c r="F57" s="18">
         <v>100</v>
       </c>
-      <c r="G40" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H40" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I40" s="18">
+      <c r="G57" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H57" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I57" s="18">
         <v>17</v>
       </c>
-      <c r="J40" s="18" t="s">
+      <c r="J57" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K40" s="18">
+      <c r="K57" s="18">
         <v>250</v>
       </c>
-      <c r="L40" s="18" t="s">
+      <c r="L57" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
+    <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="18">
+      <c r="B58" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="18">
         <v>1000</v>
       </c>
-      <c r="D41" s="18">
+      <c r="D58" s="18">
         <v>400</v>
       </c>
-      <c r="E41" s="18">
-        <v>700</v>
-      </c>
-      <c r="F41" s="18">
+      <c r="E58" s="18">
+        <v>700</v>
+      </c>
+      <c r="F58" s="18">
         <v>125</v>
       </c>
-      <c r="G41" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I41" s="18">
+      <c r="G58" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I58" s="18">
         <v>17</v>
-      </c>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18">
-        <v>250</v>
-      </c>
-      <c r="L41" s="18"/>
-    </row>
-    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="20">
-        <v>1250</v>
-      </c>
-      <c r="D42" s="18">
-        <v>400</v>
-      </c>
-      <c r="E42" s="18">
-        <v>700</v>
-      </c>
-      <c r="F42" s="18">
-        <v>150</v>
-      </c>
-      <c r="G42" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I42" s="18">
-        <v>17</v>
-      </c>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18">
-        <v>250</v>
-      </c>
-      <c r="L42" s="18"/>
-    </row>
-    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="20">
-        <v>1500</v>
-      </c>
-      <c r="D43" s="18">
-        <v>400</v>
-      </c>
-      <c r="E43" s="18">
-        <v>700</v>
-      </c>
-      <c r="F43" s="18">
-        <v>175</v>
-      </c>
-      <c r="G43" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H43" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I43" s="18">
-        <v>17</v>
-      </c>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18">
-        <v>250</v>
-      </c>
-      <c r="L43" s="18"/>
-    </row>
-    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="18">
-        <v>1500</v>
-      </c>
-      <c r="D44" s="18">
-        <v>400</v>
-      </c>
-      <c r="E44" s="18">
-        <v>700</v>
-      </c>
-      <c r="F44" s="18">
-        <v>100</v>
-      </c>
-      <c r="G44" s="19">
-        <f>G43*0.99</f>
-        <v>0.96524999999999994</v>
-      </c>
-      <c r="H44" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I44" s="18">
-        <v>17</v>
-      </c>
-      <c r="J44" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="K44" s="18">
-        <v>250</v>
-      </c>
-      <c r="L44" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" s="20">
-        <v>1750</v>
-      </c>
-      <c r="D45" s="18">
-        <v>400</v>
-      </c>
-      <c r="E45" s="18">
-        <v>700</v>
-      </c>
-      <c r="F45" s="18">
-        <v>125</v>
-      </c>
-      <c r="G45" s="19">
-        <v>0.96524999999999994</v>
-      </c>
-      <c r="H45" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I45" s="18">
-        <v>17</v>
-      </c>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18">
-        <v>250</v>
-      </c>
-      <c r="L45" s="18"/>
-    </row>
-    <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="20">
-        <v>2000</v>
-      </c>
-      <c r="D46" s="18">
-        <v>400</v>
-      </c>
-      <c r="E46" s="18">
-        <v>700</v>
-      </c>
-      <c r="F46" s="18">
-        <v>150</v>
-      </c>
-      <c r="G46" s="19">
-        <v>0.96524999999999994</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I46" s="18">
-        <v>17</v>
-      </c>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18">
-        <v>250</v>
-      </c>
-      <c r="L46" s="18"/>
-    </row>
-    <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="20">
-        <v>2250</v>
-      </c>
-      <c r="D47" s="18">
-        <v>400</v>
-      </c>
-      <c r="E47" s="18">
-        <v>700</v>
-      </c>
-      <c r="F47" s="18">
-        <v>175</v>
-      </c>
-      <c r="G47" s="19">
-        <v>0.96524999999999994</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I47" s="18">
-        <v>17</v>
-      </c>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18">
-        <v>250</v>
-      </c>
-      <c r="L47" s="18"/>
-    </row>
-    <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" s="20">
-        <v>500</v>
-      </c>
-      <c r="D48" s="20">
-        <v>700</v>
-      </c>
-      <c r="E48" s="18">
-        <v>150</v>
-      </c>
-      <c r="F48" s="18">
-        <v>20</v>
-      </c>
-      <c r="G48" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H48" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I48" s="18">
-        <v>10</v>
-      </c>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18">
-        <v>35</v>
-      </c>
-      <c r="L48" s="18"/>
-    </row>
-    <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C49" s="20">
-        <v>500</v>
-      </c>
-      <c r="D49" s="20">
-        <v>700</v>
-      </c>
-      <c r="E49" s="18">
-        <v>150</v>
-      </c>
-      <c r="F49" s="18">
-        <v>30</v>
-      </c>
-      <c r="G49" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H49" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I49" s="18">
-        <v>10</v>
-      </c>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18">
-        <v>35</v>
-      </c>
-      <c r="L49" s="18"/>
-    </row>
-    <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="20">
-        <v>500</v>
-      </c>
-      <c r="D50" s="20">
-        <v>700</v>
-      </c>
-      <c r="E50" s="18">
-        <v>150</v>
-      </c>
-      <c r="F50" s="18">
-        <v>40</v>
-      </c>
-      <c r="G50" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H50" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I50" s="18">
-        <v>10</v>
-      </c>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18">
-        <v>35</v>
-      </c>
-      <c r="L50" s="18"/>
-    </row>
-    <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="20">
-        <v>500</v>
-      </c>
-      <c r="D51" s="20">
-        <v>700</v>
-      </c>
-      <c r="E51" s="18">
-        <v>150</v>
-      </c>
-      <c r="F51" s="18">
-        <v>50</v>
-      </c>
-      <c r="G51" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I51" s="18">
-        <v>10</v>
-      </c>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18">
-        <v>35</v>
-      </c>
-      <c r="L51" s="18"/>
-    </row>
-    <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="20">
-        <v>500</v>
-      </c>
-      <c r="D52" s="20">
-        <v>700</v>
-      </c>
-      <c r="E52" s="18">
-        <v>150</v>
-      </c>
-      <c r="F52" s="18">
-        <v>20</v>
-      </c>
-      <c r="G52" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H52" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I52" s="18">
-        <v>10</v>
-      </c>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18">
-        <v>35</v>
-      </c>
-      <c r="L52" s="18"/>
-    </row>
-    <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="20">
-        <v>500</v>
-      </c>
-      <c r="D53" s="20">
-        <v>700</v>
-      </c>
-      <c r="E53" s="18">
-        <v>150</v>
-      </c>
-      <c r="F53" s="18">
-        <v>30</v>
-      </c>
-      <c r="G53" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H53" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I53" s="18">
-        <v>10</v>
-      </c>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18">
-        <v>35</v>
-      </c>
-      <c r="L53" s="18"/>
-    </row>
-    <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" s="20">
-        <v>500</v>
-      </c>
-      <c r="D54" s="20">
-        <v>700</v>
-      </c>
-      <c r="E54" s="18">
-        <v>150</v>
-      </c>
-      <c r="F54" s="18">
-        <v>40</v>
-      </c>
-      <c r="G54" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H54" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I54" s="18">
-        <v>10</v>
-      </c>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18">
-        <v>35</v>
-      </c>
-      <c r="L54" s="18"/>
-    </row>
-    <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C55" s="20">
-        <v>500</v>
-      </c>
-      <c r="D55" s="20">
-        <v>700</v>
-      </c>
-      <c r="E55" s="18">
-        <v>150</v>
-      </c>
-      <c r="F55" s="18">
-        <v>50</v>
-      </c>
-      <c r="G55" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H55" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I55" s="18">
-        <v>10</v>
-      </c>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18">
-        <v>35</v>
-      </c>
-      <c r="L55" s="18"/>
-    </row>
-    <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56" s="20">
-        <v>500</v>
-      </c>
-      <c r="D56" s="20">
-        <v>700</v>
-      </c>
-      <c r="E56" s="18">
-        <v>150</v>
-      </c>
-      <c r="F56" s="18">
-        <v>7</v>
-      </c>
-      <c r="G56" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H56" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I56" s="18">
-        <v>5</v>
-      </c>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18">
-        <v>10</v>
-      </c>
-      <c r="L56" s="18"/>
-    </row>
-    <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C57" s="20">
-        <v>500</v>
-      </c>
-      <c r="D57" s="20">
-        <v>700</v>
-      </c>
-      <c r="E57" s="18">
-        <v>150</v>
-      </c>
-      <c r="F57" s="18">
-        <v>11</v>
-      </c>
-      <c r="G57" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H57" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I57" s="18">
-        <v>5</v>
-      </c>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18">
-        <v>10</v>
-      </c>
-      <c r="L57" s="18"/>
-    </row>
-    <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C58" s="20">
-        <v>500</v>
-      </c>
-      <c r="D58" s="20">
-        <v>700</v>
-      </c>
-      <c r="E58" s="18">
-        <v>150</v>
-      </c>
-      <c r="F58" s="18">
-        <v>22</v>
-      </c>
-      <c r="G58" s="19">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H58" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I58" s="18">
-        <v>5</v>
       </c>
       <c r="J58" s="18"/>
       <c r="K58" s="18">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="L58" s="18"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="21" t="s">
-        <v>19</v>
+      <c r="A59" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C59" s="20">
-        <v>500</v>
-      </c>
-      <c r="D59" s="20">
-        <v>700</v>
+        <v>1250</v>
+      </c>
+      <c r="D59" s="18">
+        <v>400</v>
       </c>
       <c r="E59" s="18">
+        <v>700</v>
+      </c>
+      <c r="F59" s="18">
         <v>150</v>
       </c>
-      <c r="F59" s="18">
-        <v>35</v>
-      </c>
       <c r="G59" s="19">
         <v>0.97499999999999998</v>
       </c>
@@ -2692,32 +2690,32 @@
         <v>21</v>
       </c>
       <c r="I59" s="18">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J59" s="18"/>
       <c r="K59" s="18">
-        <v>35</v>
+        <v>250</v>
       </c>
       <c r="L59" s="18"/>
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="21" t="s">
-        <v>22</v>
+      <c r="A60" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="B60" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C60" s="20">
-        <v>500</v>
-      </c>
-      <c r="D60" s="20">
-        <v>350</v>
+        <v>1500</v>
+      </c>
+      <c r="D60" s="18">
+        <v>400</v>
       </c>
       <c r="E60" s="18">
-        <v>48</v>
+        <v>700</v>
       </c>
       <c r="F60" s="18">
-        <v>0.5</v>
+        <v>175</v>
       </c>
       <c r="G60" s="19">
         <v>0.97499999999999998</v>
@@ -2726,32 +2724,32 @@
         <v>21</v>
       </c>
       <c r="I60" s="18">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J60" s="18"/>
       <c r="K60" s="18">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="L60" s="18"/>
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="21" t="s">
-        <v>22</v>
+      <c r="A61" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C61" s="20">
-        <v>500</v>
-      </c>
-      <c r="D61" s="20">
-        <v>350</v>
+        <v>1500</v>
+      </c>
+      <c r="D61" s="18">
+        <v>400</v>
       </c>
       <c r="E61" s="18">
-        <v>48</v>
+        <v>700</v>
       </c>
       <c r="F61" s="18">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="G61" s="19">
         <v>0.97499999999999998</v>
@@ -2760,32 +2758,32 @@
         <v>21</v>
       </c>
       <c r="I61" s="18">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J61" s="18"/>
       <c r="K61" s="18">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="L61" s="18"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="21" t="s">
-        <v>22</v>
+      <c r="A62" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C62" s="20">
-        <v>500</v>
-      </c>
-      <c r="D62" s="20">
-        <v>350</v>
+        <v>1500</v>
+      </c>
+      <c r="D62" s="18">
+        <v>400</v>
       </c>
       <c r="E62" s="18">
-        <v>48</v>
+        <v>350</v>
       </c>
       <c r="F62" s="18">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="G62" s="19">
         <v>0.97499999999999998</v>
@@ -2794,29 +2792,29 @@
         <v>21</v>
       </c>
       <c r="I62" s="18">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J62" s="18"/>
       <c r="K62" s="18">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="L62" s="18"/>
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="21" t="s">
-        <v>22</v>
+      <c r="A63" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C63" s="20">
-        <v>500</v>
-      </c>
-      <c r="D63" s="20">
-        <v>700</v>
+        <v>1500</v>
+      </c>
+      <c r="D63" s="18">
+        <v>400</v>
       </c>
       <c r="E63" s="18">
-        <v>48</v>
+        <v>350</v>
       </c>
       <c r="F63" s="18">
         <v>11</v>
@@ -2828,188 +2826,192 @@
         <v>21</v>
       </c>
       <c r="I63" s="18">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J63" s="18"/>
       <c r="K63" s="18">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L63" s="18"/>
     </row>
     <row r="64" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="21" t="s">
-        <v>22</v>
+      <c r="A64" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="20">
-        <v>500</v>
-      </c>
-      <c r="D64" s="20">
-        <v>700</v>
+      <c r="C64" s="18">
+        <v>1500</v>
+      </c>
+      <c r="D64" s="18">
+        <v>400</v>
       </c>
       <c r="E64" s="18">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="F64" s="18">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G64" s="19">
-        <v>0.97499999999999998</v>
+        <f>G60*0.99</f>
+        <v>0.96524999999999994</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I64" s="18">
-        <v>5</v>
-      </c>
-      <c r="J64" s="18"/>
+        <v>17</v>
+      </c>
+      <c r="J64" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="K64" s="18">
-        <v>10</v>
-      </c>
-      <c r="L64" s="18"/>
+        <v>250</v>
+      </c>
+      <c r="L64" s="18" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="65" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="21" t="s">
-        <v>22</v>
+      <c r="A65" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C65" s="20">
-        <v>500</v>
-      </c>
-      <c r="D65" s="20">
-        <v>700</v>
+        <v>1750</v>
+      </c>
+      <c r="D65" s="18">
+        <v>400</v>
       </c>
       <c r="E65" s="18">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="F65" s="18">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="G65" s="19">
-        <v>0.97499999999999998</v>
+        <v>0.96524999999999994</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I65" s="18">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J65" s="18"/>
       <c r="K65" s="18">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="L65" s="18"/>
     </row>
     <row r="66" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="21" t="s">
-        <v>22</v>
+      <c r="A66" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C66" s="20">
-        <v>500</v>
-      </c>
-      <c r="D66" s="20">
-        <v>700</v>
+        <v>2000</v>
+      </c>
+      <c r="D66" s="18">
+        <v>400</v>
       </c>
       <c r="E66" s="18">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="F66" s="18">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="G66" s="19">
-        <v>0.97499999999999998</v>
+        <v>0.96524999999999994</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I66" s="18">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J66" s="18"/>
       <c r="K66" s="18">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="L66" s="18"/>
     </row>
     <row r="67" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="21" t="s">
-        <v>22</v>
+      <c r="A67" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C67" s="20">
-        <v>500</v>
-      </c>
-      <c r="D67" s="20">
-        <v>700</v>
+        <v>2250</v>
+      </c>
+      <c r="D67" s="18">
+        <v>400</v>
       </c>
       <c r="E67" s="18">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="F67" s="18">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="G67" s="19">
-        <v>0.97499999999999998</v>
+        <v>0.96524999999999994</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I67" s="18">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J67" s="18"/>
       <c r="K67" s="18">
-        <v>35</v>
+        <v>250</v>
       </c>
       <c r="L67" s="18"/>
     </row>
     <row r="68" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="21" t="s">
-        <v>23</v>
+      <c r="A68" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C68" s="20">
-        <v>500</v>
-      </c>
-      <c r="D68" s="20">
-        <v>350</v>
+        <v>1500</v>
+      </c>
+      <c r="D68" s="18">
+        <v>400</v>
       </c>
       <c r="E68" s="18">
-        <v>48</v>
+        <v>700</v>
       </c>
       <c r="F68" s="18">
-        <v>0.5</v>
+        <v>60</v>
       </c>
       <c r="G68" s="19">
-        <f>G67*0.99</f>
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I68" s="18">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J68" s="18"/>
       <c r="K68" s="18">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="L68" s="18"/>
     </row>
     <row r="69" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="21" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>20</v>
@@ -3024,13 +3026,13 @@
         <v>48</v>
       </c>
       <c r="F69" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G69" s="19">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H69" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I69" s="18">
         <v>5</v>
@@ -3043,7 +3045,7 @@
     </row>
     <row r="70" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="21" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>20</v>
@@ -3055,29 +3057,29 @@
         <v>350</v>
       </c>
       <c r="E70" s="18">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F70" s="18">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G70" s="19">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I70" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J70" s="18"/>
       <c r="K70" s="18">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="L70" s="18"/>
     </row>
     <row r="71" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="21" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>20</v>
@@ -3089,29 +3091,29 @@
         <v>700</v>
       </c>
       <c r="E71" s="18">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="F71" s="18">
         <v>11</v>
       </c>
       <c r="G71" s="19">
-        <v>0.96524999999999994</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I71" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J71" s="18"/>
       <c r="K71" s="18">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="L71" s="18"/>
     </row>
     <row r="72" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="21" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>20</v>
@@ -3123,128 +3125,1251 @@
         <v>700</v>
       </c>
       <c r="E72" s="18">
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="F72" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G72" s="19">
-        <f>G71*0.99</f>
-        <v>0.95559749999999999</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I72" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J72" s="18"/>
       <c r="K72" s="18">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="L72" s="18"/>
     </row>
     <row r="73" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="21" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="22">
-        <v>500</v>
-      </c>
-      <c r="D73" s="22">
-        <v>700</v>
-      </c>
-      <c r="E73" s="23">
-        <v>350</v>
-      </c>
-      <c r="F73" s="23">
-        <v>15</v>
-      </c>
-      <c r="G73" s="24">
-        <v>0.96524999999999994</v>
-      </c>
-      <c r="H73" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I73" s="23">
-        <v>5</v>
-      </c>
-      <c r="J73" s="23"/>
-      <c r="K73" s="23">
-        <v>10</v>
-      </c>
-      <c r="L73" s="23"/>
+      <c r="C73" s="20">
+        <v>500</v>
+      </c>
+      <c r="D73" s="20">
+        <v>700</v>
+      </c>
+      <c r="E73" s="18">
+        <v>150</v>
+      </c>
+      <c r="F73" s="18">
+        <v>20</v>
+      </c>
+      <c r="G73" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H73" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I73" s="18">
+        <v>10</v>
+      </c>
+      <c r="J73" s="18"/>
+      <c r="K73" s="18">
+        <v>35</v>
+      </c>
+      <c r="L73" s="18"/>
     </row>
     <row r="74" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" s="20">
+        <v>500</v>
+      </c>
+      <c r="D74" s="20">
+        <v>700</v>
+      </c>
+      <c r="E74" s="18">
+        <v>150</v>
+      </c>
+      <c r="F74" s="18">
+        <v>30</v>
+      </c>
+      <c r="G74" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H74" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I74" s="18">
+        <v>10</v>
+      </c>
+      <c r="J74" s="18"/>
+      <c r="K74" s="18">
+        <v>35</v>
+      </c>
+      <c r="L74" s="18"/>
+    </row>
+    <row r="75" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C75" s="20">
+        <v>500</v>
+      </c>
+      <c r="D75" s="20">
+        <v>700</v>
+      </c>
+      <c r="E75" s="18">
+        <v>150</v>
+      </c>
+      <c r="F75" s="18">
+        <v>40</v>
+      </c>
+      <c r="G75" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H75" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I75" s="18">
+        <v>10</v>
+      </c>
+      <c r="J75" s="18"/>
+      <c r="K75" s="18">
+        <v>35</v>
+      </c>
+      <c r="L75" s="18"/>
+    </row>
+    <row r="76" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="20">
+        <v>500</v>
+      </c>
+      <c r="D76" s="20">
+        <v>700</v>
+      </c>
+      <c r="E76" s="18">
+        <v>150</v>
+      </c>
+      <c r="F76" s="18">
+        <v>50</v>
+      </c>
+      <c r="G76" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I76" s="18">
+        <v>10</v>
+      </c>
+      <c r="J76" s="18"/>
+      <c r="K76" s="18">
+        <v>35</v>
+      </c>
+      <c r="L76" s="18"/>
+    </row>
+    <row r="77" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" s="20">
+        <v>500</v>
+      </c>
+      <c r="D77" s="20">
+        <v>700</v>
+      </c>
+      <c r="E77" s="18">
+        <v>150</v>
+      </c>
+      <c r="F77" s="18">
+        <v>8</v>
+      </c>
+      <c r="G77" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H77" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I77" s="18">
+        <v>10</v>
+      </c>
+      <c r="J77" s="18"/>
+      <c r="K77" s="18">
+        <v>35</v>
+      </c>
+      <c r="L77" s="18"/>
+    </row>
+    <row r="78" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" s="20">
+        <v>500</v>
+      </c>
+      <c r="D78" s="20">
+        <v>350</v>
+      </c>
+      <c r="E78" s="18">
+        <v>150</v>
+      </c>
+      <c r="F78" s="18">
+        <v>11</v>
+      </c>
+      <c r="G78" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H78" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I78" s="18">
+        <v>10</v>
+      </c>
+      <c r="J78" s="18"/>
+      <c r="K78" s="18">
+        <v>35</v>
+      </c>
+      <c r="L78" s="18"/>
+    </row>
+    <row r="79" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79" s="20">
+        <v>500</v>
+      </c>
+      <c r="D79" s="20">
+        <v>700</v>
+      </c>
+      <c r="E79" s="18">
+        <v>150</v>
+      </c>
+      <c r="F79" s="18">
+        <v>11</v>
+      </c>
+      <c r="G79" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H79" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I79" s="18">
+        <v>10</v>
+      </c>
+      <c r="J79" s="18"/>
+      <c r="K79" s="18">
+        <v>35</v>
+      </c>
+      <c r="L79" s="18"/>
+    </row>
+    <row r="80" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80" s="20">
+        <v>500</v>
+      </c>
+      <c r="D80" s="20">
+        <v>700</v>
+      </c>
+      <c r="E80" s="18">
+        <v>150</v>
+      </c>
+      <c r="F80" s="18">
+        <v>20</v>
+      </c>
+      <c r="G80" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H80" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I80" s="18">
+        <v>10</v>
+      </c>
+      <c r="J80" s="18"/>
+      <c r="K80" s="18">
+        <v>35</v>
+      </c>
+      <c r="L80" s="18"/>
+    </row>
+    <row r="81" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81" s="20">
+        <v>500</v>
+      </c>
+      <c r="D81" s="20">
+        <v>700</v>
+      </c>
+      <c r="E81" s="18">
+        <v>150</v>
+      </c>
+      <c r="F81" s="18">
+        <v>30</v>
+      </c>
+      <c r="G81" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H81" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I81" s="18">
+        <v>10</v>
+      </c>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18">
+        <v>35</v>
+      </c>
+      <c r="L81" s="18"/>
+    </row>
+    <row r="82" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" s="20">
+        <v>500</v>
+      </c>
+      <c r="D82" s="20">
+        <v>700</v>
+      </c>
+      <c r="E82" s="18">
+        <v>150</v>
+      </c>
+      <c r="F82" s="18">
+        <v>40</v>
+      </c>
+      <c r="G82" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H82" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I82" s="18">
+        <v>10</v>
+      </c>
+      <c r="J82" s="18"/>
+      <c r="K82" s="18">
+        <v>35</v>
+      </c>
+      <c r="L82" s="18"/>
+    </row>
+    <row r="83" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" s="20">
+        <v>500</v>
+      </c>
+      <c r="D83" s="20">
+        <v>700</v>
+      </c>
+      <c r="E83" s="18">
+        <v>150</v>
+      </c>
+      <c r="F83" s="18">
+        <v>50</v>
+      </c>
+      <c r="G83" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H83" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I83" s="18">
+        <v>10</v>
+      </c>
+      <c r="J83" s="18"/>
+      <c r="K83" s="18">
+        <v>35</v>
+      </c>
+      <c r="L83" s="18"/>
+    </row>
+    <row r="84" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" s="20">
+        <v>500</v>
+      </c>
+      <c r="D84" s="20">
+        <v>700</v>
+      </c>
+      <c r="E84" s="18">
+        <v>150</v>
+      </c>
+      <c r="F84" s="18">
+        <v>7</v>
+      </c>
+      <c r="G84" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H84" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I84" s="18">
+        <v>5</v>
+      </c>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18">
+        <v>10</v>
+      </c>
+      <c r="L84" s="18"/>
+    </row>
+    <row r="85" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" s="20">
+        <v>500</v>
+      </c>
+      <c r="D85" s="20">
+        <v>700</v>
+      </c>
+      <c r="E85" s="18">
+        <v>150</v>
+      </c>
+      <c r="F85" s="18">
+        <v>11</v>
+      </c>
+      <c r="G85" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H85" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I85" s="18">
+        <v>5</v>
+      </c>
+      <c r="J85" s="18"/>
+      <c r="K85" s="18">
+        <v>10</v>
+      </c>
+      <c r="L85" s="18"/>
+    </row>
+    <row r="86" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" s="20">
+        <v>500</v>
+      </c>
+      <c r="D86" s="20">
+        <v>350</v>
+      </c>
+      <c r="E86" s="18">
+        <v>150</v>
+      </c>
+      <c r="F86" s="18">
+        <v>22</v>
+      </c>
+      <c r="G86" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H86" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I86" s="18">
+        <v>5</v>
+      </c>
+      <c r="J86" s="18"/>
+      <c r="K86" s="18">
+        <v>10</v>
+      </c>
+      <c r="L86" s="18"/>
+    </row>
+    <row r="87" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C87" s="20">
+        <v>500</v>
+      </c>
+      <c r="D87" s="20">
+        <v>700</v>
+      </c>
+      <c r="E87" s="18">
+        <v>150</v>
+      </c>
+      <c r="F87" s="18">
+        <v>22</v>
+      </c>
+      <c r="G87" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H87" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I87" s="18">
+        <v>5</v>
+      </c>
+      <c r="J87" s="18"/>
+      <c r="K87" s="18">
+        <v>10</v>
+      </c>
+      <c r="L87" s="18"/>
+    </row>
+    <row r="88" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C88" s="20">
+        <v>500</v>
+      </c>
+      <c r="D88" s="20">
+        <v>700</v>
+      </c>
+      <c r="E88" s="18">
+        <v>150</v>
+      </c>
+      <c r="F88" s="18">
+        <v>35</v>
+      </c>
+      <c r="G88" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H88" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I88" s="18">
+        <v>10</v>
+      </c>
+      <c r="J88" s="18"/>
+      <c r="K88" s="18">
+        <v>35</v>
+      </c>
+      <c r="L88" s="18"/>
+    </row>
+    <row r="89" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C89" s="20">
+        <v>500</v>
+      </c>
+      <c r="D89" s="20">
+        <v>350</v>
+      </c>
+      <c r="E89" s="18">
+        <v>48</v>
+      </c>
+      <c r="F89" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="G89" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H89" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I89" s="18">
+        <v>5</v>
+      </c>
+      <c r="J89" s="18"/>
+      <c r="K89" s="18">
+        <v>10</v>
+      </c>
+      <c r="L89" s="18"/>
+    </row>
+    <row r="90" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" s="20">
+        <v>500</v>
+      </c>
+      <c r="D90" s="20">
+        <v>350</v>
+      </c>
+      <c r="E90" s="18">
+        <v>48</v>
+      </c>
+      <c r="F90" s="18">
+        <v>1</v>
+      </c>
+      <c r="G90" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H90" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I90" s="18">
+        <v>5</v>
+      </c>
+      <c r="J90" s="18"/>
+      <c r="K90" s="18">
+        <v>5</v>
+      </c>
+      <c r="L90" s="18"/>
+    </row>
+    <row r="91" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C91" s="20">
+        <v>500</v>
+      </c>
+      <c r="D91" s="20">
+        <v>350</v>
+      </c>
+      <c r="E91" s="18">
+        <v>48</v>
+      </c>
+      <c r="F91" s="18">
+        <v>3</v>
+      </c>
+      <c r="G91" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H91" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I91" s="18">
+        <v>5</v>
+      </c>
+      <c r="J91" s="18"/>
+      <c r="K91" s="18">
+        <v>5</v>
+      </c>
+      <c r="L91" s="18"/>
+    </row>
+    <row r="92" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C92" s="20">
+        <v>500</v>
+      </c>
+      <c r="D92" s="20">
+        <v>350</v>
+      </c>
+      <c r="E92" s="18">
+        <v>48</v>
+      </c>
+      <c r="F92" s="18">
+        <v>5</v>
+      </c>
+      <c r="G92" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H92" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I92" s="18">
+        <v>5</v>
+      </c>
+      <c r="J92" s="18"/>
+      <c r="K92" s="18">
+        <v>5</v>
+      </c>
+      <c r="L92" s="18"/>
+    </row>
+    <row r="93" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C93" s="20">
+        <v>500</v>
+      </c>
+      <c r="D93" s="20">
+        <v>350</v>
+      </c>
+      <c r="E93" s="18">
+        <v>48</v>
+      </c>
+      <c r="F93" s="18">
+        <v>6</v>
+      </c>
+      <c r="G93" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H93" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I93" s="18">
+        <v>5</v>
+      </c>
+      <c r="J93" s="18"/>
+      <c r="K93" s="18">
+        <v>5</v>
+      </c>
+      <c r="L93" s="18"/>
+    </row>
+    <row r="94" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C94" s="20">
+        <v>500</v>
+      </c>
+      <c r="D94" s="20">
+        <v>700</v>
+      </c>
+      <c r="E94" s="18">
+        <v>48</v>
+      </c>
+      <c r="F94" s="18">
+        <v>11</v>
+      </c>
+      <c r="G94" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H94" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I94" s="18">
+        <v>5</v>
+      </c>
+      <c r="J94" s="18"/>
+      <c r="K94" s="18">
+        <v>10</v>
+      </c>
+      <c r="L94" s="18"/>
+    </row>
+    <row r="95" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" s="20">
+        <v>500</v>
+      </c>
+      <c r="D95" s="20">
+        <v>700</v>
+      </c>
+      <c r="E95" s="18">
+        <v>350</v>
+      </c>
+      <c r="F95" s="18">
+        <v>10</v>
+      </c>
+      <c r="G95" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H95" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I95" s="18">
+        <v>5</v>
+      </c>
+      <c r="J95" s="18"/>
+      <c r="K95" s="18">
+        <v>10</v>
+      </c>
+      <c r="L95" s="18"/>
+    </row>
+    <row r="96" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C96" s="20">
+        <v>500</v>
+      </c>
+      <c r="D96" s="20">
+        <v>700</v>
+      </c>
+      <c r="E96" s="18">
+        <v>350</v>
+      </c>
+      <c r="F96" s="18">
+        <v>15</v>
+      </c>
+      <c r="G96" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H96" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I96" s="18">
+        <v>5</v>
+      </c>
+      <c r="J96" s="18"/>
+      <c r="K96" s="18">
+        <v>10</v>
+      </c>
+      <c r="L96" s="18"/>
+    </row>
+    <row r="97" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C97" s="20">
+        <v>500</v>
+      </c>
+      <c r="D97" s="20">
+        <v>700</v>
+      </c>
+      <c r="E97" s="18">
+        <v>350</v>
+      </c>
+      <c r="F97" s="18">
+        <v>20</v>
+      </c>
+      <c r="G97" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H97" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I97" s="18">
+        <v>5</v>
+      </c>
+      <c r="J97" s="18"/>
+      <c r="K97" s="18">
+        <v>10</v>
+      </c>
+      <c r="L97" s="18"/>
+    </row>
+    <row r="98" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C98" s="20">
+        <v>500</v>
+      </c>
+      <c r="D98" s="20">
+        <v>700</v>
+      </c>
+      <c r="E98" s="18">
+        <v>350</v>
+      </c>
+      <c r="F98" s="18">
+        <v>50</v>
+      </c>
+      <c r="G98" s="19">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H98" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I98" s="18">
+        <v>10</v>
+      </c>
+      <c r="J98" s="18"/>
+      <c r="K98" s="18">
+        <v>35</v>
+      </c>
+      <c r="L98" s="18"/>
+    </row>
+    <row r="99" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B74" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C74" s="16">
-        <v>500</v>
-      </c>
-      <c r="D74" s="16">
-        <v>700</v>
-      </c>
-      <c r="E74" s="14">
-        <v>350</v>
-      </c>
-      <c r="F74" s="14">
-        <v>20</v>
-      </c>
-      <c r="G74" s="15">
+      <c r="B99" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" s="20">
+        <v>500</v>
+      </c>
+      <c r="D99" s="20">
+        <v>350</v>
+      </c>
+      <c r="E99" s="18">
+        <v>48</v>
+      </c>
+      <c r="F99" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="G99" s="19">
+        <f>G98*0.99</f>
         <v>0.96524999999999994</v>
       </c>
-      <c r="H74" s="14" t="s">
+      <c r="H99" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I74" s="14">
-        <v>10</v>
-      </c>
-      <c r="J74" s="14"/>
-      <c r="K74" s="14">
+      <c r="I99" s="18">
+        <v>5</v>
+      </c>
+      <c r="J99" s="18"/>
+      <c r="K99" s="18">
+        <v>5</v>
+      </c>
+      <c r="L99" s="18"/>
+    </row>
+    <row r="100" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" s="20">
+        <v>500</v>
+      </c>
+      <c r="D100" s="20">
+        <v>350</v>
+      </c>
+      <c r="E100" s="18">
+        <v>48</v>
+      </c>
+      <c r="F100" s="18">
+        <v>1</v>
+      </c>
+      <c r="G100" s="19">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H100" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I100" s="18">
+        <v>5</v>
+      </c>
+      <c r="J100" s="18"/>
+      <c r="K100" s="18">
+        <v>5</v>
+      </c>
+      <c r="L100" s="18"/>
+    </row>
+    <row r="101" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C101" s="20">
+        <v>500</v>
+      </c>
+      <c r="D101" s="20">
+        <v>350</v>
+      </c>
+      <c r="E101" s="18">
+        <v>48</v>
+      </c>
+      <c r="F101" s="18">
+        <v>3</v>
+      </c>
+      <c r="G101" s="19">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H101" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I101" s="18">
+        <v>5</v>
+      </c>
+      <c r="J101" s="18"/>
+      <c r="K101" s="18">
+        <v>5</v>
+      </c>
+      <c r="L101" s="18"/>
+    </row>
+    <row r="102" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C102" s="20">
+        <v>500</v>
+      </c>
+      <c r="D102" s="20">
+        <v>350</v>
+      </c>
+      <c r="E102" s="18">
+        <v>48</v>
+      </c>
+      <c r="F102" s="18">
+        <v>5</v>
+      </c>
+      <c r="G102" s="19">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H102" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I102" s="18">
+        <v>5</v>
+      </c>
+      <c r="J102" s="18"/>
+      <c r="K102" s="18">
+        <v>5</v>
+      </c>
+      <c r="L102" s="18"/>
+    </row>
+    <row r="103" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C103" s="20">
+        <v>500</v>
+      </c>
+      <c r="D103" s="20">
+        <v>350</v>
+      </c>
+      <c r="E103" s="18">
+        <v>48</v>
+      </c>
+      <c r="F103" s="18">
+        <v>6</v>
+      </c>
+      <c r="G103" s="19">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H103" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I103" s="18">
+        <v>5</v>
+      </c>
+      <c r="J103" s="18"/>
+      <c r="K103" s="18">
+        <v>5</v>
+      </c>
+      <c r="L103" s="18"/>
+    </row>
+    <row r="104" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C104" s="20">
+        <v>500</v>
+      </c>
+      <c r="D104" s="20">
+        <v>700</v>
+      </c>
+      <c r="E104" s="18">
+        <v>48</v>
+      </c>
+      <c r="F104" s="18">
+        <v>11</v>
+      </c>
+      <c r="G104" s="19">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H104" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I104" s="18">
+        <v>5</v>
+      </c>
+      <c r="J104" s="18"/>
+      <c r="K104" s="18">
+        <v>10</v>
+      </c>
+      <c r="L104" s="18"/>
+    </row>
+    <row r="105" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C105" s="20">
+        <v>500</v>
+      </c>
+      <c r="D105" s="20">
+        <v>700</v>
+      </c>
+      <c r="E105" s="18">
+        <v>350</v>
+      </c>
+      <c r="F105" s="18">
+        <v>10</v>
+      </c>
+      <c r="G105" s="19">
+        <f>G104*0.99</f>
+        <v>0.95559749999999999</v>
+      </c>
+      <c r="H105" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I105" s="18">
+        <v>5</v>
+      </c>
+      <c r="J105" s="18"/>
+      <c r="K105" s="18">
+        <v>10</v>
+      </c>
+      <c r="L105" s="18"/>
+    </row>
+    <row r="106" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C106" s="22">
+        <v>500</v>
+      </c>
+      <c r="D106" s="22">
+        <v>700</v>
+      </c>
+      <c r="E106" s="23">
+        <v>350</v>
+      </c>
+      <c r="F106" s="23">
+        <v>15</v>
+      </c>
+      <c r="G106" s="24">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H106" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I106" s="23">
+        <v>5</v>
+      </c>
+      <c r="J106" s="23"/>
+      <c r="K106" s="23">
+        <v>10</v>
+      </c>
+      <c r="L106" s="23"/>
+    </row>
+    <row r="107" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C107" s="16">
+        <v>500</v>
+      </c>
+      <c r="D107" s="16">
+        <v>700</v>
+      </c>
+      <c r="E107" s="14">
+        <v>350</v>
+      </c>
+      <c r="F107" s="14">
+        <v>20</v>
+      </c>
+      <c r="G107" s="15">
+        <v>0.96524999999999994</v>
+      </c>
+      <c r="H107" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I107" s="14">
+        <v>10</v>
+      </c>
+      <c r="J107" s="14"/>
+      <c r="K107" s="14">
         <v>35</v>
       </c>
-      <c r="L74" s="14"/>
-    </row>
-    <row r="75" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="25" t="s">
+      <c r="L107" s="14"/>
+    </row>
+    <row r="108" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B75" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C75" s="16">
-        <v>500</v>
-      </c>
-      <c r="D75" s="16">
-        <v>700</v>
-      </c>
-      <c r="E75" s="14">
-        <v>350</v>
-      </c>
-      <c r="F75" s="14">
+      <c r="B108" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C108" s="16">
+        <v>500</v>
+      </c>
+      <c r="D108" s="16">
+        <v>700</v>
+      </c>
+      <c r="E108" s="14">
+        <v>350</v>
+      </c>
+      <c r="F108" s="14">
         <v>50</v>
       </c>
-      <c r="G75" s="15">
+      <c r="G108" s="15">
         <v>0.96524999999999994</v>
       </c>
-      <c r="H75" s="14" t="s">
+      <c r="H108" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I75" s="14">
-        <v>10</v>
-      </c>
-      <c r="J75" s="14"/>
-      <c r="K75" s="14">
+      <c r="I108" s="14">
+        <v>10</v>
+      </c>
+      <c r="J108" s="14"/>
+      <c r="K108" s="14">
         <v>35</v>
       </c>
-      <c r="L75" s="14"/>
+      <c r="L108" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>